<commit_message>
Updating whole folder structure
</commit_message>
<xml_diff>
--- a/Excel_Output/Hotel_Details.xlsx
+++ b/Excel_Output/Hotel_Details.xlsx
@@ -26,28 +26,28 @@
     <t>Elegant Cosy Conquest</t>
   </si>
   <si>
-    <t>₹ 8,315</t>
+    <t>₹ 8,401</t>
   </si>
   <si>
-    <t>₹ 41,578 / 5 nights</t>
+    <t>₹ 42,009 / 5 nights</t>
   </si>
   <si>
     <t>City/River View Retreat in the Heart of Westlands</t>
   </si>
   <si>
-    <t>₹ 5,987</t>
+    <t>₹ 6,049</t>
   </si>
   <si>
-    <t>₹ 29,936 / 5 nights</t>
+    <t>₹ 30,246 / 5 nights</t>
   </si>
   <si>
     <t>Holiday Apartment 5 Rooms Junction Mall Nairobi</t>
   </si>
   <si>
-    <t>₹ 9,147</t>
+    <t>₹ 9,242</t>
   </si>
   <si>
-    <t>₹ 45,736 / 5 nights</t>
+    <t>₹ 46,210 / 5 nights</t>
   </si>
 </sst>
 </file>

</xml_diff>